<commit_message>
Dossier de remise finale du tp2
</commit_message>
<xml_diff>
--- a/tp2/GrapheLinearPerfectHashing.xlsx
+++ b/tp2/GrapheLinearPerfectHashing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\paulc\github\inf2010\tp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A5F3A7-9E37-4E15-8ECC-E829F08D4E6F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED6988F-41A1-4A57-9599-D48D320EA65C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{4B4819B4-9909-45AA-BCC3-06BE5024E854}"/>
+    <workbookView xWindow="2805" yWindow="3150" windowWidth="10920" windowHeight="8400" xr2:uid="{4B4819B4-9909-45AA-BCC3-06BE5024E854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CA"/>
-              <a:t>Graphe de 3 test</a:t>
+              <a:t>Graphe de 3 tests</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="fr-CA" baseline="0"/>
@@ -3336,8 +3336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5E177A7-98DF-469B-9E52-FD5A50175865}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D40" sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>